<commit_message>
Hoàn thiện xóa học sinh: khóa tài khoản, thông báo rõ ràng, nhập/xuất Excel thành công.
</commit_message>
<xml_diff>
--- a/Student-Management-System_CSharp_SGU2025/ConnectDatabase/SampleData_Import_updated.xlsx
+++ b/Student-Management-System_CSharp_SGU2025/ConnectDatabase/SampleData_Import_updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HocSinh" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Mã HS</t>
   </si>
@@ -55,19 +55,16 @@
     <t/>
   </si>
   <si>
-    <t>Nguyễn Văn Tèo</t>
-  </si>
-  <si>
-    <t>15/05/2008</t>
+    <t>Lương Con A</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>0912349999</t>
-  </si>
-  <si>
-    <t>teo.nguyen@student.edu.vn</t>
+    <t>0912349889</t>
+  </si>
+  <si>
+    <t>conluon@student.edu.vn</t>
   </si>
   <si>
     <t>Đang học</t>
@@ -85,16 +82,16 @@
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>Nguyễn Văn Téo</t>
-  </si>
-  <si>
-    <t>0901234576</t>
-  </si>
-  <si>
-    <t>nguyen.van.teo@gmail.com</t>
-  </si>
-  <si>
-    <t>456 Huệ, Q5, TP.HCM</t>
+    <t>Lương Chúa A</t>
+  </si>
+  <si>
+    <t>0901237584</t>
+  </si>
+  <si>
+    <t>luongChua@gmail.com</t>
+  </si>
+  <si>
+    <t>485 ZZZ, Q7, TP.HCM</t>
   </si>
   <si>
     <t>Học Sinh</t>
@@ -119,7 +116,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,22 +135,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,157 +586,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1096,11 +1087,19 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="12.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="26.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -1132,20 +1131,20 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3">
+        <v>39485</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1165,7 +1164,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="teo.nguyen@student.edu.vn"/>
+    <hyperlink ref="F2" r:id="rId1" display="conluon@student.edu.vn" tooltip="mailto:conluon@student.edu.vn"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1177,27 +1176,33 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="25.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="21.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1205,16 +1210,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1239,7 +1244,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="nguyen.van.teo@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="luongChua@gmail.com" tooltip="mailto:luongChua@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1252,20 +1257,25 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="17.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="14.8571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1273,10 +1283,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hoàn thiện xóa học sinh: khóa tài khoản, thông báo rõ ràng, nhập/xuất Excel thành công. (#58)
Co-authored-by: nuyntai19 <tuantai1915@gmail.com>
</commit_message>
<xml_diff>
--- a/Student-Management-System_CSharp_SGU2025/ConnectDatabase/SampleData_Import_updated.xlsx
+++ b/Student-Management-System_CSharp_SGU2025/ConnectDatabase/SampleData_Import_updated.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="HocSinh" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>Mã HS</t>
   </si>
@@ -55,19 +55,16 @@
     <t/>
   </si>
   <si>
-    <t>Nguyễn Văn Tèo</t>
-  </si>
-  <si>
-    <t>15/05/2008</t>
+    <t>Lương Con A</t>
   </si>
   <si>
     <t>Nam</t>
   </si>
   <si>
-    <t>0912349999</t>
-  </si>
-  <si>
-    <t>teo.nguyen@student.edu.vn</t>
+    <t>0912349889</t>
+  </si>
+  <si>
+    <t>conluon@student.edu.vn</t>
   </si>
   <si>
     <t>Đang học</t>
@@ -85,16 +82,16 @@
     <t>Địa chỉ</t>
   </si>
   <si>
-    <t>Nguyễn Văn Téo</t>
-  </si>
-  <si>
-    <t>0901234576</t>
-  </si>
-  <si>
-    <t>nguyen.van.teo@gmail.com</t>
-  </si>
-  <si>
-    <t>456 Huệ, Q5, TP.HCM</t>
+    <t>Lương Chúa A</t>
+  </si>
+  <si>
+    <t>0901237584</t>
+  </si>
+  <si>
+    <t>luongChua@gmail.com</t>
+  </si>
+  <si>
+    <t>485 ZZZ, Q7, TP.HCM</t>
   </si>
   <si>
     <t>Học Sinh</t>
@@ -119,7 +116,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,22 +135,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -596,157 +586,158 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1096,11 +1087,19 @@
   <sheetPr/>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="2" max="2" width="12.2857142857143" customWidth="1"/>
+    <col min="3" max="3" width="12.8571428571429" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="13.5714285714286" customWidth="1"/>
+    <col min="6" max="6" width="26.1428571428571" customWidth="1"/>
+    <col min="7" max="7" width="15.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
@@ -1132,20 +1131,20 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3">
+        <v>39485</v>
+      </c>
+      <c r="D2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1">
@@ -1165,7 +1164,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="teo.nguyen@student.edu.vn"/>
+    <hyperlink ref="F2" r:id="rId1" display="conluon@student.edu.vn" tooltip="mailto:conluon@student.edu.vn"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1177,27 +1176,33 @@
   <sheetPr/>
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="4"/>
+  <cols>
+    <col min="2" max="2" width="13.8571428571429" customWidth="1"/>
+    <col min="3" max="3" width="13.5714285714286" customWidth="1"/>
+    <col min="4" max="4" width="25.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="21.4285714285714" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1205,16 +1210,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
-      </c>
-      <c r="E2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -1239,7 +1244,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="nguyen.van.teo@gmail.com"/>
+    <hyperlink ref="D2" r:id="rId1" display="luongChua@gmail.com" tooltip="mailto:luongChua@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1252,20 +1257,25 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="17.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="14.8571428571429" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1273,10 +1283,10 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>